<commit_message>
August 6 - requirement trace cleanup
A few adjustments in the requirements and tests to improve their flow.
</commit_message>
<xml_diff>
--- a/review/Features Requirement Check.xlsx
+++ b/review/Features Requirement Check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\GitHub\oapi_common\review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE62738-BFB3-4347-B35F-0221E4C6047F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DBDCF7-541A-440B-A0AF-23F1A1353193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="2454" windowWidth="17280" windowHeight="8994" xr2:uid="{820C61C1-A234-4EA0-91F4-C3B848BDCD06}"/>
+    <workbookView xWindow="1230" yWindow="450" windowWidth="17280" windowHeight="8994" activeTab="1" xr2:uid="{820C61C1-A234-4EA0-91F4-C3B848BDCD06}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="145">
   <si>
     <t>API-Features</t>
   </si>
@@ -412,12 +412,6 @@
     <t>Part 1</t>
   </si>
   <si>
-    <t>The requirements are equivalent - Common also specifies that the Collection resource schema should be used.</t>
-  </si>
-  <si>
-    <t>Common also specifies the schema to be used.</t>
-  </si>
-  <si>
     <t>Common includes D and E from fc-bbox-response and adds CRS84H for 3-D.</t>
   </si>
   <si>
@@ -464,6 +458,15 @@
   </si>
   <si>
     <t>Could use a little more refinement</t>
+  </si>
+  <si>
+    <t>The requirements are equivalent - Common also includes a Collection Requirements Module which makes validation of the collection resource a single referenceable package</t>
+  </si>
+  <si>
+    <t>/req/collections/collection-definition</t>
+  </si>
+  <si>
+    <t>Makes (conceptual) conformance with the JSON schema an explicit requirement.</t>
   </si>
 </sst>
 </file>
@@ -859,7 +862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D20426A-668C-46BF-8B70-867F7C0CABFC}">
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="B47" sqref="B47:B48"/>
     </sheetView>
   </sheetViews>
@@ -1290,7 +1293,7 @@
         <v>35</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1301,7 +1304,7 @@
         <v>35</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1312,7 +1315,7 @@
         <v>35</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1524,10 +1527,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B76526C-0D11-40AA-B8CC-4F9CFBEE45A2}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B45" sqref="B45:B47"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1691,10 +1694,10 @@
         <v>102</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
@@ -1702,7 +1705,7 @@
         <v>103</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1713,7 +1716,7 @@
         <v>104</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1724,7 +1727,7 @@
         <v>105</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1735,7 +1738,7 @@
         <v>106</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1749,7 +1752,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -1757,169 +1760,169 @@
         <v>109</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="4" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>76</v>
+        <v>143</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="4" t="s">
-        <v>140</v>
-      </c>
       <c r="B29" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>141</v>
+        <v>76</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="4" t="s">
+      <c r="B31" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>112</v>
-      </c>
       <c r="C33" s="4" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>74</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="4" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>132</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1927,10 +1930,10 @@
         <v>76</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1938,142 +1941,153 @@
         <v>76</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>134</v>
+      <c r="C43" s="5" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>137</v>
+      <c r="C45" s="6" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="3" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C54" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="56" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Features Requirements Check spreadsheet
</commit_message>
<xml_diff>
--- a/review/Features Requirement Check.xlsx
+++ b/review/Features Requirement Check.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\GitHub\oapi_common\review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DBDCF7-541A-440B-A0AF-23F1A1353193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5059F654-0041-4E1C-B830-FD9753DF59A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="450" windowWidth="17280" windowHeight="8994" activeTab="1" xr2:uid="{820C61C1-A234-4EA0-91F4-C3B848BDCD06}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8994" activeTab="1" xr2:uid="{820C61C1-A234-4EA0-91F4-C3B848BDCD06}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="143">
   <si>
     <t>API-Features</t>
   </si>
@@ -345,15 +345,6 @@
     <t>/req/collections/rc-md-items</t>
   </si>
   <si>
-    <t>/req/collections/rc-bbox-unsupported</t>
-  </si>
-  <si>
-    <t>/req/collections/rc-datetime-unsupported</t>
-  </si>
-  <si>
-    <t>/req/collections/rc-limit-unsupported</t>
-  </si>
-  <si>
     <t>Simple Query Requirements Class</t>
   </si>
   <si>
@@ -394,9 +385,6 @@
   </si>
   <si>
     <t>/req/collections/rc-limit-collection-response</t>
-  </si>
-  <si>
-    <t>/req/collections/rc-paged-response</t>
   </si>
   <si>
     <t>/req/collections/rc-numberMatched</t>
@@ -433,9 +421,6 @@
     <t>The requirements are equivalent but apply to different resources (/collections vs. /collections/{collectionid}/items).</t>
   </si>
   <si>
-    <t>Consider making this a recommendation in Common</t>
-  </si>
-  <si>
     <t>This is the /collections/{collectionid}/items end point</t>
   </si>
   <si>
@@ -445,9 +430,6 @@
     <t>The requirements are identical but apply to different resources (/collections vs. /collections/{collectionid}/items).</t>
   </si>
   <si>
-    <t>Consider deleting from Common</t>
-  </si>
-  <si>
     <t>TBR</t>
   </si>
   <si>
@@ -457,9 +439,6 @@
     <t>Feature mandates links to the items in the collection. This is a Feature-specific requirement</t>
   </si>
   <si>
-    <t>Could use a little more refinement</t>
-  </si>
-  <si>
     <t>The requirements are equivalent - Common also includes a Collection Requirements Module which makes validation of the collection resource a single referenceable package</t>
   </si>
   <si>
@@ -467,6 +446,21 @@
   </si>
   <si>
     <t>Makes (conceptual) conformance with the JSON schema an explicit requirement.</t>
+  </si>
+  <si>
+    <t>/req/collections/rc-dependency-http</t>
+  </si>
+  <si>
+    <t>Collections can stand alone so this requirement needs to be re-stated</t>
+  </si>
+  <si>
+    <t>The requirements are equivalent in the context of Feature Collections.</t>
+  </si>
+  <si>
+    <t>/rec/collections/rc-paged-response</t>
+  </si>
+  <si>
+    <t>Was a requirement - note invalid URI.</t>
   </si>
 </sst>
 </file>
@@ -1218,7 +1212,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1293,7 +1287,7 @@
         <v>35</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1304,7 +1298,7 @@
         <v>35</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1315,7 +1309,7 @@
         <v>35</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1527,10 +1521,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B76526C-0D11-40AA-B8CC-4F9CFBEE45A2}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1565,7 +1559,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1573,7 +1567,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1581,7 +1575,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1589,7 +1583,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1597,7 +1591,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1605,7 +1599,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1618,7 +1612,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1626,7 +1620,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1634,7 +1628,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1655,21 +1649,21 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>99</v>
+        <v>76</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>74</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>74</v>
@@ -1677,252 +1671,252 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="4" t="s">
+      <c r="C19" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>137</v>
+      <c r="C20" s="4" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C21" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>137</v>
+      <c r="C22" s="4" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="4" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="4" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>143</v>
+        <v>76</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="4" t="s">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B33" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>128</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="C39" s="4" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1930,165 +1924,144 @@
         <v>76</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>130</v>
+        <v>141</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="4" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C42" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>132</v>
+        <v>35</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>135</v>
+      <c r="A47" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>135</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>38</v>
+      <c r="A49" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C54" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="54" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>